<commit_message>
Revert "Revert "sms template""
This reverts commit c1093a021b9c1702809f368a794515f04c871773.
</commit_message>
<xml_diff>
--- a/public/process_variables.xlsx
+++ b/public/process_variables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
   <si>
     <t>VAR_ID</t>
   </si>
@@ -104,12 +104,30 @@
     <t>integer</t>
   </si>
   <si>
+    <t>310614396652148af08f122080329400</t>
+  </si>
+  <si>
+    <t>agency_manager_national_id</t>
+  </si>
+  <si>
     <t>32406339064e34dce406b64089642611</t>
   </si>
   <si>
     <t>substitute</t>
   </si>
   <si>
+    <t>38980047265214996a96853053294934</t>
+  </si>
+  <si>
+    <t>inactivity_commitment_image</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>97290740465214979a6b891095846179</t>
+  </si>
+  <si>
     <t>477146009652119e56206b8097951634</t>
   </si>
   <si>
@@ -218,6 +236,21 @@
     <t>warning_receiver</t>
   </si>
   <si>
+    <t>92013649665214880f338a7062586547</t>
+  </si>
+  <si>
+    <t>referral</t>
+  </si>
+  <si>
+    <t>[{"value":"1","label":"\u0645\u0631\u0627\u062c\u0639\u0647 \u06a9\u0631\u062f"},{"value":"0","label":"\u0645\u0631\u0627\u062c\u0639\u0647 \u0646\u06a9\u0631\u062f"}]</t>
+  </si>
+  <si>
+    <t>9244949946521480773d796066448722</t>
+  </si>
+  <si>
+    <t>referral_and_notice_sms</t>
+  </si>
+  <si>
     <t>94172160065211a796e7149060650444</t>
   </si>
   <si>
@@ -231,6 +264,15 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>995623521652147b8e3e140020518509</t>
+  </si>
+  <si>
+    <t>inactivity_commitment</t>
+  </si>
+  <si>
+    <t>[{"value":"1","label":"\u062f\u0627\u0631\u062f"},{"value":"0","label":"\u0646\u062f\u0627\u0631\u062f"}]</t>
   </si>
 </sst>
 </file>
@@ -569,7 +611,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -778,16 +820,16 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -816,16 +858,16 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -854,31 +896,31 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H8">
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="J8" t="s">
         <v>19</v>
@@ -888,35 +930,38 @@
       </c>
       <c r="N8" t="s">
         <v>20</v>
+      </c>
+      <c r="O8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -925,21 +970,21 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -968,31 +1013,31 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="J11" t="s">
         <v>19</v>
@@ -1001,24 +1046,24 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
         <v>18</v>
@@ -1044,19 +1089,19 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
@@ -1077,15 +1122,15 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -1094,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -1120,19 +1165,19 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
@@ -1153,24 +1198,24 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
         <v>18</v>
@@ -1196,31 +1241,31 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="G17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="J17" t="s">
         <v>19</v>
@@ -1234,19 +1279,19 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>
@@ -1272,10 +1317,10 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1284,19 +1329,19 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
@@ -1305,24 +1350,24 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -1348,10 +1393,10 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
@@ -1360,19 +1405,19 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="J21" t="s">
         <v>19</v>
@@ -1381,15 +1426,15 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1398,7 +1443,7 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F22" t="s">
         <v>18</v>
@@ -1424,31 +1469,31 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="J23" t="s">
         <v>19</v>
@@ -1462,19 +1507,19 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
         <v>18</v>
@@ -1500,40 +1545,230 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
         <v>9</v>
       </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
         <v>26</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="N25" t="s">
-        <v>20</v>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>